<commit_message>
added neucode pairs test
</commit_message>
<xml_diff>
--- a/Test/UnitTestFiles/noisy.xlsx
+++ b/Test/UnitTestFiles/noisy.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1343" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1355" uniqueCount="151">
   <si>
     <t xml:space="preserve">No. </t>
   </si>
@@ -472,6 +472,12 @@
   <si>
     <t>45.190-45.450</t>
   </si>
+  <si>
+    <t>362-364</t>
+  </si>
+  <si>
+    <t>49.830-50.100</t>
+  </si>
 </sst>
 </file>
 
@@ -797,10 +803,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K1280"/>
+  <dimension ref="A1:K1289"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1246" workbookViewId="0">
-      <selection activeCell="B1257" sqref="B1257"/>
+    <sheetView tabSelected="1" topLeftCell="A1255" workbookViewId="0">
+      <selection activeCell="G1287" sqref="G1287"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23411,6 +23417,174 @@
         <v>9043.7682999999997</v>
       </c>
     </row>
+    <row r="1281" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1281">
+        <v>223</v>
+      </c>
+      <c r="B1281" s="3">
+        <v>12085.651900000001</v>
+      </c>
+      <c r="C1281" s="2">
+        <v>250841.25</v>
+      </c>
+      <c r="D1281">
+        <v>3</v>
+      </c>
+      <c r="E1281">
+        <v>1</v>
+      </c>
+      <c r="F1281">
+        <v>3043.5305000000008</v>
+      </c>
+      <c r="G1281" s="3">
+        <v>0.37711287672319926</v>
+      </c>
+      <c r="H1281" s="3">
+        <v>3.8888479196368146E-3</v>
+      </c>
+      <c r="I1281" t="s">
+        <v>149</v>
+      </c>
+      <c r="J1281" t="s">
+        <v>150</v>
+      </c>
+      <c r="K1281" s="4">
+        <v>49.966163333333334</v>
+      </c>
+    </row>
+    <row r="1282" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B1282" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1282" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1282" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1282" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1283" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B1283">
+        <v>16</v>
+      </c>
+      <c r="C1283" s="2">
+        <v>1697055.24</v>
+      </c>
+      <c r="D1283" s="1">
+        <v>756.35986000000014</v>
+      </c>
+      <c r="E1283" s="3">
+        <v>12085.6517</v>
+      </c>
+    </row>
+    <row r="1284" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B1284">
+        <v>17</v>
+      </c>
+      <c r="C1284" s="2">
+        <v>1751303.34</v>
+      </c>
+      <c r="D1284" s="1">
+        <v>711.92735999999991</v>
+      </c>
+      <c r="E1284" s="3">
+        <v>12085.654500000001</v>
+      </c>
+    </row>
+    <row r="1285" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B1285">
+        <v>18</v>
+      </c>
+      <c r="C1285" s="2">
+        <v>751634.25</v>
+      </c>
+      <c r="D1285" s="1">
+        <v>672.43179999999995</v>
+      </c>
+      <c r="E1285" s="3">
+        <v>12085.645699999999</v>
+      </c>
+    </row>
+    <row r="1286" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1286">
+        <v>224</v>
+      </c>
+      <c r="B1286" s="3">
+        <v>12083.662199999999</v>
+      </c>
+      <c r="C1286" s="2">
+        <v>99194.09</v>
+      </c>
+      <c r="D1286">
+        <v>2</v>
+      </c>
+      <c r="E1286">
+        <v>1</v>
+      </c>
+      <c r="F1286">
+        <v>3041.5407999999989</v>
+      </c>
+      <c r="G1286" s="3">
+        <v>0.14912765995959568</v>
+      </c>
+      <c r="H1286" s="3">
+        <v>1.5378281304879759E-3</v>
+      </c>
+      <c r="I1286" t="s">
+        <v>149</v>
+      </c>
+      <c r="J1286" t="s">
+        <v>150</v>
+      </c>
+      <c r="K1286" s="4">
+        <v>49.966163333333334</v>
+      </c>
+    </row>
+    <row r="1287" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B1287" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1287" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1287" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1287" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1288" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B1288">
+        <v>16</v>
+      </c>
+      <c r="C1288" s="2">
+        <v>958571.49</v>
+      </c>
+      <c r="D1288" s="1">
+        <v>756.23458000000005</v>
+      </c>
+      <c r="E1288" s="3">
+        <v>12083.659600000001</v>
+      </c>
+    </row>
+    <row r="1289" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B1289">
+        <v>17</v>
+      </c>
+      <c r="C1289" s="2">
+        <v>667817.32999999996</v>
+      </c>
+      <c r="D1289" s="1">
+        <v>711.80944</v>
+      </c>
+      <c r="E1289" s="3">
+        <v>12083.661400000001</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>